<commit_message>
Worked on notebook an got new metrics
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\ICESI\SEMESTRE11\IA\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEBBA32-5BC4-4BA2-955F-A9700A41F883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8529CB3-CE2E-49C4-8341-C7EAE0FE2377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="knn" sheetId="1" r:id="rId1"/>
     <sheet name="RF" sheetId="2" r:id="rId2"/>
     <sheet name="NN" sheetId="4" r:id="rId3"/>
-    <sheet name="Comparación" sheetId="3" r:id="rId4"/>
+    <sheet name="Comparación1" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
   <si>
     <t>0.3 - 123. n=36</t>
   </si>
@@ -117,6 +118,15 @@
   </si>
   <si>
     <t>All attributes</t>
+  </si>
+  <si>
+    <t>(minmaxscaler)</t>
+  </si>
+  <si>
+    <t>n=31</t>
+  </si>
+  <si>
+    <t>n=24</t>
   </si>
 </sst>
 </file>
@@ -410,9 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -428,6 +435,14 @@
     <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -443,16 +458,9 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,7 +479,9 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,7 +1267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6D48F6-6181-46C2-9894-C8FA8EBDF562}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="M1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1267,35 +1277,35 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="11" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="14" t="s">
+      <c r="L3" s="43"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="17" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="17"/>
+      <c r="R3" s="45"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1322,21 +1332,21 @@
       <c r="K4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="20"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="O4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="19" t="s">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1344,63 +1354,63 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>0.503</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>0.45700000000000002</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="33">
         <f>ABS(B5-C5)</f>
         <v>4.5999999999999985E-2</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>0.54700000000000004</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.44600000000000001</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="33">
         <f>ABS(E5-F5)</f>
         <v>0.10100000000000003</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>0.50800000000000001</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <v>0.439</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="33">
         <f>ABS(H5-I5)</f>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
         <v>0.61199999999999999</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <v>0.42799999999999999</v>
       </c>
-      <c r="M5" s="40">
+      <c r="M5" s="33">
         <f>ABS(K5-L5)</f>
         <v>0.184</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5" s="28">
         <v>0.502</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="29">
         <v>0.47</v>
       </c>
-      <c r="P5" s="40">
+      <c r="P5" s="33">
         <f>ABS(N5-O5)</f>
         <v>3.2000000000000028E-2</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="30">
         <v>0.503</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="31">
         <v>0.47699999999999998</v>
       </c>
-      <c r="S5" s="38">
+      <c r="S5" s="32">
         <f>ABS(Q5-R5)</f>
         <v>2.6000000000000023E-2</v>
       </c>
@@ -1409,63 +1419,63 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>0.23699999999999999</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>0.16900000000000001</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="33">
         <f t="shared" ref="D6:D8" si="0">ABS(B6-C6)</f>
         <v>6.7999999999999977E-2</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>0.45100000000000001</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>0.17799999999999999</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="33">
         <f t="shared" ref="G6:G8" si="1">ABS(E6-F6)</f>
         <v>0.27300000000000002</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="24">
         <v>0.214</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>0.16800000000000001</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="33">
         <f t="shared" ref="J6:J8" si="2">ABS(H6-I6)</f>
         <v>4.5999999999999985E-2</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="26">
         <v>0.42299999999999999</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <v>0.19500000000000001</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6" s="33">
         <f t="shared" ref="M6:M8" si="3">ABS(K6-L6)</f>
         <v>0.22799999999999998</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="28">
         <v>0.214</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="29">
         <v>0.184</v>
       </c>
-      <c r="P6" s="40">
+      <c r="P6" s="33">
         <f t="shared" ref="P6:P8" si="4">ABS(N6-O6)</f>
         <v>0.03</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="30">
         <v>0.21</v>
       </c>
-      <c r="R6" s="32">
+      <c r="R6" s="31">
         <v>0.224</v>
       </c>
-      <c r="S6" s="38">
+      <c r="S6" s="32">
         <f t="shared" ref="S6:S8" si="5">ABS(Q6-R6)</f>
         <v>1.4000000000000012E-2</v>
       </c>
@@ -1474,63 +1484,63 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>0.189</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>0.16700000000000001</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="33">
         <f t="shared" si="0"/>
         <v>2.1999999999999992E-2</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>0.23200000000000001</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>0.17199999999999999</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="33">
         <f t="shared" si="1"/>
         <v>6.0000000000000026E-2</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="24">
         <v>0.193</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>0.16600000000000001</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="33">
         <f t="shared" si="2"/>
         <v>2.6999999999999996E-2</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="26">
         <v>0.30499999999999999</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
         <v>0.182</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="33">
         <f t="shared" si="3"/>
         <v>0.123</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="28">
         <v>0.188</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="29">
         <v>0.17299999999999999</v>
       </c>
-      <c r="P7" s="40">
+      <c r="P7" s="33">
         <f t="shared" si="4"/>
         <v>1.5000000000000013E-2</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="30">
         <v>0.193</v>
       </c>
-      <c r="R7" s="32">
+      <c r="R7" s="31">
         <v>0.21099999999999999</v>
       </c>
-      <c r="S7" s="38">
+      <c r="S7" s="32">
         <f t="shared" si="5"/>
         <v>1.7999999999999988E-2</v>
       </c>
@@ -1539,69 +1549,66 @@
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>0.17699999999999999</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>0.154</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="33">
         <f t="shared" si="0"/>
         <v>2.2999999999999993E-2</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>0.24</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="33">
         <f t="shared" si="1"/>
         <v>7.4999999999999983E-2</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="24">
         <v>0.186</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="25">
         <v>0.154</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="33">
         <f t="shared" si="2"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="26">
         <v>0.32400000000000001</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <v>0.18099999999999999</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="33">
         <f t="shared" si="3"/>
         <v>0.14300000000000002</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="28">
         <v>0.17599999999999999</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="29">
         <v>0.16200000000000001</v>
       </c>
-      <c r="P8" s="40">
+      <c r="P8" s="33">
         <f t="shared" si="4"/>
         <v>1.3999999999999985E-2</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="30">
         <v>0.184</v>
       </c>
-      <c r="R8" s="32">
+      <c r="R8" s="31">
         <v>0.20200000000000001</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8" s="32">
         <f t="shared" si="5"/>
         <v>1.8000000000000016E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G9" s="41"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1631,12 +1638,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1657,24 +1664,24 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="45"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>0.55700000000000005</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>0.53400000000000003</v>
       </c>
       <c r="E6">
@@ -1683,10 +1690,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>0.26</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>0.26900000000000002</v>
       </c>
       <c r="E7">
@@ -1695,10 +1702,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>0.21299999999999999</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>0.22500000000000001</v>
       </c>
       <c r="E8">
@@ -1707,10 +1714,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>0.20699999999999999</v>
       </c>
       <c r="E9">
@@ -1797,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0E7BC5-2AB5-4ECE-A19D-F18A8E7155A0}">
   <dimension ref="B1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:N9"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,54 +1818,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52" t="s">
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="34" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="15" t="s">
@@ -1872,29 +1884,29 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>0.503</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>0.47699999999999998</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <f>ABS(C6-D6)</f>
         <v>2.6000000000000023E-2</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="43">
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="35">
         <v>0.55700000000000005</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="35">
         <v>0.53400000000000003</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="35">
         <f>ABS(I6-J6)</f>
         <v>2.300000000000002E-2</v>
       </c>
@@ -1904,123 +1916,397 @@
       <c r="M6" s="16">
         <v>0.51500000000000001</v>
       </c>
+      <c r="N6" s="52">
+        <f>ABS(L6-M6)</f>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.224</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" ref="E7:E9" si="0">ABS(C7-D7)</f>
+        <v>1.4000000000000012E-2</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="35">
+        <v>0.26</v>
+      </c>
+      <c r="J7" s="35">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="K7" s="35">
+        <f t="shared" ref="K7:K9" si="1">ABS(I7-J7)</f>
+        <v>9.000000000000008E-3</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="N7" s="52">
+        <f t="shared" ref="N7:N9" si="2">ABS(L7-M7)</f>
+        <v>2.9999999999999971E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.193</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999988E-2</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="35">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="J8" s="35">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K8" s="35">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.254</v>
+      </c>
+      <c r="N8" s="52">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.184</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000016E-2</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="35">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="J9" s="35">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="K9" s="35">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0.246</v>
+      </c>
+      <c r="N9" s="52">
+        <f t="shared" si="2"/>
+        <v>1.7999999999999988E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F433D37B-1DE8-4291-8660-7AA08758F8C9}">
+  <dimension ref="B1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="E6" s="20">
+        <f>ABS(C6-D6)</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="F6" s="53">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="G6" s="53">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="H6" s="53">
+        <f>ABS(F6-G6)</f>
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="I6" s="35">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="J6" s="35">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="K6" s="35">
+        <f>ABS(I6-J6)</f>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="L6" s="28">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="M6" s="28">
+        <v>0.54700000000000004</v>
+      </c>
       <c r="N6" s="54">
         <f>ABS(L6-M6)</f>
+        <v>1.5999999999999903E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" ref="E7:E9" si="0">ABS(C7-D7)</f>
+        <v>0.123</v>
+      </c>
+      <c r="F7" s="53">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="G7" s="53">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="H7" s="53">
+        <f t="shared" ref="H7:H9" si="1">ABS(F7-G7)</f>
+        <v>4.1000000000000009E-2</v>
+      </c>
+      <c r="I7" s="35">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="J7" s="35">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="K7" s="35">
+        <f t="shared" ref="K7:K9" si="2">ABS(I7-J7)</f>
         <v>1.4000000000000012E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="21">
-        <v>0.21</v>
-      </c>
-      <c r="D7" s="21">
-        <v>0.224</v>
-      </c>
-      <c r="E7" s="21">
-        <f t="shared" ref="E7:E9" si="0">ABS(C7-D7)</f>
+      <c r="L7" s="28">
+        <v>0.314</v>
+      </c>
+      <c r="M7" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="N7" s="54">
+        <f t="shared" ref="N7:N9" si="3">ABS(L7-M7)</f>
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.253</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="F8" s="53">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="G8" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="53">
+        <f t="shared" si="1"/>
+        <v>3.9000000000000007E-2</v>
+      </c>
+      <c r="I8" s="35">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="J8" s="35">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="K8" s="35">
+        <f t="shared" si="2"/>
         <v>1.4000000000000012E-2</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="43">
-        <v>0.26</v>
-      </c>
-      <c r="J7" s="43">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="K7" s="43">
-        <f t="shared" ref="K7:K9" si="1">ABS(I7-J7)</f>
-        <v>9.000000000000008E-3</v>
-      </c>
-      <c r="L7" s="16">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="M7" s="16">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="N7" s="54">
-        <f t="shared" ref="N7:N9" si="2">ABS(L7-M7)</f>
-        <v>2.9999999999999971E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="21">
-        <v>0.193</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="L8" s="28">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="M8" s="28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N8" s="54">
+        <f t="shared" si="3"/>
+        <v>3.6000000000000032E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.249</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>1.100000000000001E-2</v>
+      </c>
+      <c r="F9" s="53">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G9" s="53">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="H9" s="53">
+        <f t="shared" si="1"/>
+        <v>3.9000000000000007E-2</v>
+      </c>
+      <c r="I9" s="35">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="J9" s="35">
         <v>0.21099999999999999</v>
       </c>
-      <c r="E8" s="21">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999988E-2</v>
-      </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="43">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="J8" s="43">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="K8" s="43">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000011E-2</v>
-      </c>
-      <c r="L8" s="16">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="M8" s="16">
-        <v>0.254</v>
-      </c>
-      <c r="N8" s="54">
+      <c r="K9" s="35">
         <f t="shared" si="2"/>
-        <v>2.6999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="21">
-        <v>0.184</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="E9" s="21">
-        <f t="shared" si="0"/>
-        <v>1.8000000000000016E-2</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="43">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="J9" s="43">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="K9" s="43">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000018E-3</v>
-      </c>
-      <c r="L9" s="16">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="M9" s="16">
-        <v>0.246</v>
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="L9" s="28">
+        <v>0.249</v>
+      </c>
+      <c r="M9" s="28">
+        <v>0.28999999999999998</v>
       </c>
       <c r="N9" s="54">
-        <f t="shared" si="2"/>
-        <v>1.7999999999999988E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.0999999999999981E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cross validation for some models
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\ICESI\SEMESTRE11\IA\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\ICESI\IA\LABORATORIO\Lab3\Lab-3-IA-2023-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8529CB3-CE2E-49C4-8341-C7EAE0FE2377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D65E0-67F5-4D86-9B25-6A81A64CE406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" firstSheet="1" activeTab="4" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="knn" sheetId="1" r:id="rId1"/>
     <sheet name="RF" sheetId="2" r:id="rId2"/>
     <sheet name="NN" sheetId="4" r:id="rId3"/>
     <sheet name="Comparación1" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
+    <sheet name="Comparacion2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -392,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -443,6 +443,10 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,9 +460,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -479,9 +480,6 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1269,45 +1267,45 @@
   <sheetViews>
     <sheetView topLeftCell="M1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="41"/>
+      <c r="F3" s="43"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="42"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="43"/>
+      <c r="L3" s="45"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="44"/>
+      <c r="O3" s="46"/>
       <c r="P3" s="14"/>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="45"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R3" s="41"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1415,7 +1413,7 @@
         <v>2.6000000000000023E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1480,7 +1478,7 @@
         <v>1.4000000000000012E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1543,7 @@
         <v>1.7999999999999988E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>1.8000000000000016E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1632,7 +1630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
@@ -1658,18 +1656,18 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="45"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="41"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="30">
         <v>0.55700000000000005</v>
       </c>
@@ -1689,7 +1687,7 @@
         <v>2.300000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C7" s="30">
         <v>0.26</v>
       </c>
@@ -1701,7 +1699,7 @@
         <v>9.000000000000008E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C8" s="30">
         <v>0.21299999999999999</v>
       </c>
@@ -1713,7 +1711,7 @@
         <v>1.2000000000000011E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" s="30">
         <v>0.20499999999999999</v>
       </c>
@@ -1742,19 +1740,19 @@
       <selection activeCell="B8" sqref="B8:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>0.52900000000000003</v>
       </c>
@@ -1770,7 +1768,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>0.28599999999999998</v>
       </c>
@@ -1778,7 +1776,7 @@
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>0.22700000000000001</v>
       </c>
@@ -1786,7 +1784,7 @@
         <v>0.254</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>0.22800000000000001</v>
       </c>
@@ -1808,9 +1806,9 @@
       <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>23</v>
       </c>
@@ -1818,34 +1816,34 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="46" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50" t="s">
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="51" t="s">
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
@@ -1883,7 +1881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="39" t="s">
         <v>8</v>
       </c>
@@ -1916,12 +1914,12 @@
       <c r="M6" s="16">
         <v>0.51500000000000001</v>
       </c>
-      <c r="N6" s="52">
+      <c r="N6" s="16">
         <f>ABS(L6-M6)</f>
         <v>1.4000000000000012E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="39" t="s">
         <v>9</v>
       </c>
@@ -1954,12 +1952,12 @@
       <c r="M7" s="16">
         <v>0.25600000000000001</v>
       </c>
-      <c r="N7" s="52">
+      <c r="N7" s="16">
         <f t="shared" ref="N7:N9" si="2">ABS(L7-M7)</f>
         <v>2.9999999999999971E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="39" t="s">
         <v>10</v>
       </c>
@@ -1992,12 +1990,12 @@
       <c r="M8" s="16">
         <v>0.254</v>
       </c>
-      <c r="N8" s="52">
+      <c r="N8" s="16">
         <f t="shared" si="2"/>
         <v>2.6999999999999996E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="39" t="s">
         <v>11</v>
       </c>
@@ -2030,7 +2028,7 @@
       <c r="M9" s="16">
         <v>0.246</v>
       </c>
-      <c r="N9" s="52">
+      <c r="N9" s="16">
         <f t="shared" si="2"/>
         <v>1.7999999999999988E-2</v>
       </c>
@@ -2050,13 +2048,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F433D37B-1DE8-4291-8660-7AA08758F8C9}">
   <dimension ref="B1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>23</v>
       </c>
@@ -2064,34 +2062,34 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="46" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50" t="s">
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="51" t="s">
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
@@ -2129,7 +2127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="39" t="s">
         <v>8</v>
       </c>
@@ -2143,13 +2141,13 @@
         <f>ABS(C6-D6)</f>
         <v>3.499999999999992E-2</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="40">
         <v>0.54200000000000004</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="40">
         <v>0.54800000000000004</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="40">
         <f>ABS(F6-G6)</f>
         <v>6.0000000000000053E-3</v>
       </c>
@@ -2169,12 +2167,12 @@
       <c r="M6" s="28">
         <v>0.54700000000000004</v>
       </c>
-      <c r="N6" s="54">
+      <c r="N6" s="28">
         <f>ABS(L6-M6)</f>
         <v>1.5999999999999903E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="39" t="s">
         <v>9</v>
       </c>
@@ -2188,13 +2186,13 @@
         <f t="shared" ref="E7:E9" si="0">ABS(C7-D7)</f>
         <v>0.123</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="40">
         <v>0.23200000000000001</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="40">
         <v>0.27300000000000002</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="40">
         <f t="shared" ref="H7:H9" si="1">ABS(F7-G7)</f>
         <v>4.1000000000000009E-2</v>
       </c>
@@ -2214,12 +2212,12 @@
       <c r="M7" s="28">
         <v>0.375</v>
       </c>
-      <c r="N7" s="54">
+      <c r="N7" s="28">
         <f t="shared" ref="N7:N9" si="3">ABS(L7-M7)</f>
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="39" t="s">
         <v>10</v>
       </c>
@@ -2233,13 +2231,13 @@
         <f t="shared" si="0"/>
         <v>1.5000000000000013E-2</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="40">
         <v>0.21099999999999999</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="40">
         <v>0.25</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="40">
         <f t="shared" si="1"/>
         <v>3.9000000000000007E-2</v>
       </c>
@@ -2259,12 +2257,12 @@
       <c r="M8" s="28">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N8" s="54">
+      <c r="N8" s="28">
         <f t="shared" si="3"/>
         <v>3.6000000000000032E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="39" t="s">
         <v>11</v>
       </c>
@@ -2278,13 +2276,13 @@
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="40">
         <v>0.20499999999999999</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="40">
         <v>0.24399999999999999</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="40">
         <f t="shared" si="1"/>
         <v>3.9000000000000007E-2</v>
       </c>
@@ -2304,7 +2302,7 @@
       <c r="M9" s="28">
         <v>0.28999999999999998</v>
       </c>
-      <c r="N9" s="54">
+      <c r="N9" s="28">
         <f t="shared" si="3"/>
         <v>4.0999999999999981E-2</v>
       </c>

</xml_diff>

<commit_message>
added comparison per class
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\ICESI\IA\LABORATORIO\Lab3\Lab-3-IA-2023-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953FF94F-C61C-4695-8CE5-4EC51864EDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB94F30-E8C6-4F56-AD9C-056C42344AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="740" windowWidth="10280" windowHeight="7360" firstSheet="1" activeTab="4" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="knn" sheetId="1" r:id="rId1"/>
     <sheet name="RF" sheetId="2" r:id="rId2"/>
     <sheet name="NN" sheetId="4" r:id="rId3"/>
-    <sheet name="Comparación1" sheetId="3" r:id="rId4"/>
-    <sheet name="Comparacion2" sheetId="5" r:id="rId5"/>
+    <sheet name="ComparacionPorClases" sheetId="6" r:id="rId4"/>
+    <sheet name="ComparaciónSinEscalar" sheetId="3" r:id="rId5"/>
+    <sheet name="ComparacionEscalado" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
   <si>
     <t>0.3 - 123. n=36</t>
   </si>
@@ -127,6 +128,27 @@
   </si>
   <si>
     <t>n=24</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>PRECISION</t>
+  </si>
+  <si>
+    <t>RECALL</t>
+  </si>
+  <si>
+    <t>F1-SCORE</t>
+  </si>
+  <si>
+    <t>ACCURACY</t>
   </si>
 </sst>
 </file>
@@ -509,6 +531,3564 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Precisión por clase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$C$2:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>PRECISION</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF05-4C64-AB77-637D03DAAC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$D$2:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>PRECISION</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AF05-4C64-AB77-637D03DAAC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$E$2:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>PRECISION</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AF05-4C64-AB77-637D03DAAC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$F$2:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>PRECISION</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$F$4:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AF05-4C64-AB77-637D03DAAC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="727631296"/>
+        <c:axId val="855644736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="727631296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="855644736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="855644736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="727631296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Recall por clase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$C$19:$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RECALL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$21:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$C$21:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC08-4D9E-889B-C7FA0843B444}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$D$19:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RECALL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$21:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$D$21:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AC08-4D9E-889B-C7FA0843B444}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$E$19:$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RECALL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$21:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$E$21:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AC08-4D9E-889B-C7FA0843B444}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$F$19:$F$20</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RECALL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$21:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$F$21:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AC08-4D9E-889B-C7FA0843B444}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="727597696"/>
+        <c:axId val="852617376"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="727597696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852617376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="852617376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="727597696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>F1 por clase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$C$34:$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>F1-SCORE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$36:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$C$36:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8D2-4BE8-91A7-418B6ECD96C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$D$34:$D$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>F1-SCORE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$36:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$D$36:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B8D2-4BE8-91A7-418B6ECD96C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$E$34:$E$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>F1-SCORE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$36:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$E$36:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B8D2-4BE8-91A7-418B6ECD96C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ComparacionPorClases!$F$34:$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>F1-SCORE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$B$36:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ComparacionPorClases!$F$36:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B8D2-4BE8-91A7-418B6ECD96C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="727608736"/>
+        <c:axId val="887592960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="727608736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="887592960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="887592960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="727608736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,6 +4546,119 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE54492-8E11-0919-A066-5FA828749FCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5B8CEB-3969-1841-CF95-7630C7EBD67E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D50931E-5976-C380-5617-C414458BEBBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1799,10 +5492,426 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D68EAC7-CB22-4037-A75A-1C6B45CDFD7D}">
+  <dimension ref="B2:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.59</v>
+      </c>
+      <c r="E6">
+        <v>0.59</v>
+      </c>
+      <c r="F6">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.53</v>
+      </c>
+      <c r="D7">
+        <v>0.53</v>
+      </c>
+      <c r="E7">
+        <v>0.51</v>
+      </c>
+      <c r="F7">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.49</v>
+      </c>
+      <c r="D8">
+        <v>0.52</v>
+      </c>
+      <c r="E8">
+        <v>0.53</v>
+      </c>
+      <c r="F8">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D23">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E23">
+        <v>0.46</v>
+      </c>
+      <c r="F23">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>0.72</v>
+      </c>
+      <c r="D24">
+        <v>0.75</v>
+      </c>
+      <c r="E24">
+        <v>0.83</v>
+      </c>
+      <c r="F24">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+      <c r="D25">
+        <v>0.18</v>
+      </c>
+      <c r="E25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D38">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E38">
+        <v>0.52</v>
+      </c>
+      <c r="F38">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>0.61</v>
+      </c>
+      <c r="D39">
+        <v>0.62</v>
+      </c>
+      <c r="E39">
+        <v>0.63</v>
+      </c>
+      <c r="F39">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>0.33</v>
+      </c>
+      <c r="D40">
+        <v>0.27</v>
+      </c>
+      <c r="E40">
+        <v>0.12</v>
+      </c>
+      <c r="F40">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48">
+        <v>0.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0E7BC5-2AB5-4ECE-A19D-F18A8E7155A0}">
   <dimension ref="B1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
@@ -2044,11 +6153,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F433D37B-1DE8-4291-8660-7AA08758F8C9}">
   <dimension ref="B1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="B3" zoomScale="116" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tried with only class 5,6,7
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\ICESI\IA\LABORATORIO\Lab3\Lab-3-IA-2023-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB94F30-E8C6-4F56-AD9C-056C42344AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26454B63-C1C8-4962-852C-1FE56F30C83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{D0D0DE32-06C9-4B46-950C-413F0A1F8EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="knn" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ComparacionPorClases" sheetId="6" r:id="rId4"/>
     <sheet name="ComparaciónSinEscalar" sheetId="3" r:id="rId5"/>
     <sheet name="ComparacionEscalado" sheetId="5" r:id="rId6"/>
+    <sheet name="ComparacionQuitandoClases" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="38">
   <si>
     <t>0.3 - 123. n=36</t>
   </si>
@@ -149,6 +150,12 @@
   </si>
   <si>
     <t>ACCURACY</t>
+  </si>
+  <si>
+    <t>(usando todas las clases de quality)</t>
+  </si>
+  <si>
+    <t>(usando solo las clases 5,6,7 de quality)</t>
   </si>
 </sst>
 </file>
@@ -4191,8 +4198,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>589718</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>184546</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1984</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4958,13 +4965,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6D48F6-6181-46C2-9894-C8FA8EBDF562}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="AL1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -5343,15 +5355,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A250F6-7791-4D27-A3A1-08EE43893014}">
-  <dimension ref="A4:E9"/>
+  <dimension ref="A4:G9"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -5359,8 +5371,11 @@
         <v>16</v>
       </c>
       <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
@@ -5368,7 +5383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="30">
         <v>0.55700000000000005</v>
       </c>
@@ -5380,7 +5395,7 @@
         <v>2.300000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" s="30">
         <v>0.26</v>
       </c>
@@ -5392,7 +5407,7 @@
         <v>9.000000000000008E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C8" s="30">
         <v>0.21299999999999999</v>
       </c>
@@ -5404,7 +5419,7 @@
         <v>1.2000000000000011E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C9" s="30">
         <v>0.20499999999999999</v>
       </c>
@@ -5430,7 +5445,7 @@
   <dimension ref="A4:C11"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5438,6 +5453,9 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -5493,20 +5511,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D68EAC7-CB22-4037-A75A-1C6B45CDFD7D}">
-  <dimension ref="B2:F48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>18</v>
       </c>
@@ -5520,7 +5541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>3</v>
       </c>
@@ -5537,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>4</v>
       </c>
@@ -5554,7 +5575,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>5</v>
       </c>
@@ -5571,7 +5592,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>6</v>
       </c>
@@ -5588,7 +5609,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>7</v>
       </c>
@@ -5605,7 +5626,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>8</v>
       </c>
@@ -5912,7 +5933,7 @@
   <dimension ref="B1:N9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5923,6 +5944,9 @@
       </c>
       <c r="E1" t="s">
         <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
@@ -6157,8 +6181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F433D37B-1DE8-4291-8660-7AA08758F8C9}">
   <dimension ref="B1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="116" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="N9" sqref="B4:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6170,6 +6194,9 @@
       <c r="E1" t="s">
         <v>26</v>
       </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
@@ -6418,6 +6445,243 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="M10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6D2BA1-2C86-4EFA-B30C-8D7D7C52548C}">
+  <dimension ref="B1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C4" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C5" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E6" s="20">
+        <f>ABS(C6-D6)</f>
+        <v>2.9000000000000026E-2</v>
+      </c>
+      <c r="F6" s="40">
+        <v>0.59</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H6" s="40">
+        <f>ABS(F6-G6)</f>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35">
+        <f>ABS(I6-J6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28">
+        <f>ABS(L6-M6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" ref="E7:E13" si="0">ABS(C7-D7)</f>
+        <v>6.6000000000000059E-2</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="H7" s="40">
+        <f t="shared" ref="H7:H9" si="1">ABS(F7-G7)</f>
+        <v>2.1000000000000019E-2</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35">
+        <f t="shared" ref="K7:K9" si="2">ABS(I7-J7)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28">
+        <f t="shared" ref="N7:N9" si="3">ABS(L7-M7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>4.500000000000004E-2</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.51</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="H8" s="40">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000024E-2</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>4.7999999999999932E-2</v>
+      </c>
+      <c r="F9" s="40">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="G9" s="40">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H9" s="40">
+        <f t="shared" si="1"/>
+        <v>3.1000000000000028E-2</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>